<commit_message>
Editing my personal information
</commit_message>
<xml_diff>
--- a/Fondos de Inversion.xlsx
+++ b/Fondos de Inversion.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2244,10 +2244,8 @@
           <t>Renta Acciones</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>252000001274</t>
-        </is>
+      <c r="C49" t="n">
+        <v>252000001274</v>
       </c>
       <c r="D49" t="n">
         <v>64235.41601415</v>
@@ -2283,10 +2281,8 @@
           <t>Fidurenta</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>1111000544148</t>
-        </is>
+      <c r="C50" t="n">
+        <v>1111000544148</v>
       </c>
       <c r="D50" t="n">
         <v>44938.25051329</v>
@@ -2322,10 +2318,8 @@
           <t>Renta Fija Plazo</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>252000011589</t>
-        </is>
+      <c r="C51" t="n">
+        <v>252000011589</v>
       </c>
       <c r="D51" t="n">
         <v>36011.2935991</v>
@@ -2361,10 +2355,8 @@
           <t>Fiducuenta</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>342000006519</t>
-        </is>
+      <c r="C52" t="n">
+        <v>342000006519</v>
       </c>
       <c r="D52" t="n">
         <v>38949.69336621</v>
@@ -2389,6 +2381,162 @@
       </c>
       <c r="K52" t="n">
         <v>12.01</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Fidurenta</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>1111000544148</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>45233.36324127</v>
+      </c>
+      <c r="E53" t="n">
+        <v>119590.77</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>-133.75</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>119457.02</v>
+      </c>
+      <c r="K53" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Renta Acciones</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>252000001274</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>70711.08490446</v>
+      </c>
+      <c r="E54" t="n">
+        <v>779626.88</v>
+      </c>
+      <c r="F54" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>-147388.81</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>6632238.07</v>
+      </c>
+      <c r="K54" t="n">
+        <v>20.62</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Renta Fija Plazo</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>252000011589</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>35671.28200578</v>
+      </c>
+      <c r="E55" t="n">
+        <v>9256619.279999999</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="H55" t="n">
+        <v>-130131.73</v>
+      </c>
+      <c r="I55" t="n">
+        <v>2871.7</v>
+      </c>
+      <c r="J55" t="n">
+        <v>3123615.85</v>
+      </c>
+      <c r="K55" t="n">
+        <v>13.57</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Fiducuenta</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>342000006519</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>39507.92241913</v>
+      </c>
+      <c r="E56" t="n">
+        <v>596031.51</v>
+      </c>
+      <c r="F56" t="n">
+        <v>2404134</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1589059</v>
+      </c>
+      <c r="H56" t="n">
+        <v>8401.42</v>
+      </c>
+      <c r="I56" t="n">
+        <v>74.31999999999999</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1419433.61</v>
+      </c>
+      <c r="K56" t="n">
+        <v>6.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>